<commit_message>
Ajout de l'aide dans le html
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thib\unif local\Projet python\Création enigme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49B5B1B-031F-4192-B9BF-25C9EB6C834E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D83899F-7B67-4B46-8717-AC9A7E70FDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>Chap</t>
   </si>
@@ -215,6 +215,26 @@
   </si>
   <si>
     <t>Si tu écris un texte, n'oublie pas les "</t>
+  </si>
+  <si>
+    <t>En python, pour écrire un message dans la console
+On utilise la fonction print()
+ainsi, pour utiliser cette fonction, on fera par exemple :
+print("HelloWorld")
+Tu peux voir que les " sont importants, ils permettent de dire qu'il sagit d'un texte</t>
+  </si>
+  <si>
+    <t>En python, pour récuperer un message de quelqu'un dans la console
+on utilisera la fonction input()
+ainsi on fera par exemple
+message = input()
+Attention le message ici sera considéré comme un texte
+Pour preciser qu'il s'agit d'un nombre entier, on utilisera la fonction int()
+On aura ainsi
+nombre = int(input())
+ici, la variable nombre aura alors la valeur entrée par l'utilisateur
+Si jamais on a besoin de stoquer une deuxieme valeur, on utilisera alors une autre variable
+nombre2 = int(input())</t>
   </si>
 </sst>
 </file>
@@ -598,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="97" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,6 +720,9 @@
       <c r="C2">
         <v>0</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="I2" t="s">
         <v>32</v>
       </c>
@@ -732,6 +755,9 @@
       </c>
       <c r="C3">
         <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
correction bug + ajout quete incendie
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8273939F-6F08-4B16-9266-48D85252A2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D571B6F6-ED90-4F0C-A544-253EB4127EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
   <si>
     <t>Chap</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t>print("Je vais bien")</t>
-  </si>
-  <si>
-    <t>Compte les champignons pour savoir combien vous en avez</t>
   </si>
   <si>
     <t>Il faudra additionner les trois nombres</t>
@@ -297,6 +294,133 @@
     <t>625
 8.333333333333334
 5</t>
+  </si>
+  <si>
+    <t>Compte les champignons pour savoir combien vous en avez
+Il y a ici 3 types de champignons</t>
+  </si>
+  <si>
+    <t>1
+5
+4
+2
+2
+3
+2
+1
+6
+4
+5
+2
+5
+2
+3
+1
+4
+6
+3
+1</t>
+  </si>
+  <si>
+    <t>Il faut apporter 4000mL d'eau pour la maison 1
+Il faut apporter 1200mL d'eau pour la maison 2
+Il faut apporter 24000mL d'eau pour la maison 3
+Il faut apporter 3000mL d'eau pour la maison 4
+Il faut apporter 7200mL d'eau pour la maison 5
+Il faut apporter 39400mL d'eau au total</t>
+  </si>
+  <si>
+    <t>2
+4
+6
+2
+1
+3
+2
+1
+5
+4
+5
+2
+6
+2
+3
+1
+4
+6
+2
+1</t>
+  </si>
+  <si>
+    <t>1
+1
+1
+2
+2
+3
+2
+1
+1
+4
+5
+2
+7
+2
+3
+1
+5
+6
+3
+2</t>
+  </si>
+  <si>
+    <t>Il faut apporter 9600mL d'eau pour la maison 1
+Il faut apporter 600mL d'eau pour la maison 2
+Il faut apporter 20000mL d'eau pour la maison 3
+Il faut apporter 3600mL d'eau pour la maison 4
+Il faut apporter 4800mL d'eau pour la maison 5
+Il faut apporter 38600mL d'eau au total</t>
+  </si>
+  <si>
+    <t>Il faut apporter 200mL d'eau pour la maison 1
+Il faut apporter 1200mL d'eau pour la maison 2
+Il faut apporter 4000mL d'eau pour la maison 3
+Il faut apporter 4200mL d'eau pour la maison 4
+Il faut apporter 18000mL d'eau pour la maison 5
+Il faut apporter 27600mL d'eau au total</t>
+  </si>
+  <si>
+    <t>Multiplie chacune des valeurs pour obtenir le volume de flamme à éteindre</t>
+  </si>
+  <si>
+    <t>Mutliplie le resultat par 100 pour obtenir la quantité d'eau</t>
+  </si>
+  <si>
+    <t>Voici une solution possible pour une maison
+p_f_1 = int(input())
+x_m_1 = int(input())
+y_m_1 = int(input())
+z_m_1 = int(input())
+eau_1 = p_f_1*x_m_1*y_m_1*z_m_1
+print(f"Il faut apporter {eau_1*100}mL d'eau pour la maison 1")
+Ensuite calcule la somme d'eau</t>
+  </si>
+  <si>
+    <t>Arrete l'incendie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vite tu dois arreter l'incendie
+Il y a 5 maisons mais tu ne sais pas a l'avance quelle quantité d'eau tu as besoin
+Navi est partie te dire l'étendue des flammes pendant que tu es parti cherché de l'eau
+Navi te dire les informations dans l'ordre suivant:
+la puissance des flammes
+la longueur de la maison
+la largeur de la maison
+la nombre d'étage de la maison
+Elle répetera ces informations pour les 5 maisons
+Après chaque maison, tu devras lui dire quel quantité d'eau ammener
+Une fois les 5 maisons éteintes, tu devras annoncer quel quantité d'eau vous avez utilisés
+Une maison avec un incendie de puissance 1, de longueur 1, de largeur 1 et de 1 étage demandera 100mL d'eau </t>
   </si>
 </sst>
 </file>
@@ -343,7 +467,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M4" zoomScale="97" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="97" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -695,506 +821,620 @@
     <col min="20" max="20" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>0</v>
       </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L2" t="s">
+      <c r="J2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N2" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q2">
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1">
         <v>1</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
     </row>
     <row r="3" spans="1:25" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="H3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="1">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1">
+        <v>4</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I3">
+      <c r="S3" s="1">
         <v>6</v>
       </c>
-      <c r="J3">
+      <c r="T3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="1">
         <v>7</v>
       </c>
-      <c r="K3">
+      <c r="V3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="1">
         <v>14</v>
       </c>
-      <c r="L3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3">
-        <v>4</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S3">
-        <v>6</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U3">
-        <v>7</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="W3">
-        <v>14</v>
-      </c>
       <c r="X3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Y3" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:25" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1">
+        <v>3</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+    </row>
+    <row r="5" spans="1:25" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1">
+        <v>16</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1">
+        <v>4</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1">
+        <v>8</v>
+      </c>
+      <c r="U5" s="1">
+        <v>141</v>
+      </c>
+      <c r="V5" s="1">
+        <v>10</v>
+      </c>
+      <c r="W5" s="1">
+        <v>226</v>
+      </c>
+      <c r="X5" s="1">
+        <v>15</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="216" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1">
+        <v>4</v>
+      </c>
+      <c r="R6" s="1">
+        <v>2</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="T6" s="1">
+        <v>3</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="V6" s="1">
+        <v>5</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="X6" s="1">
+        <v>25</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1">
+        <v>8</v>
+      </c>
+      <c r="J7" s="1">
+        <v>27</v>
+      </c>
+      <c r="K7" s="1">
+        <v>64</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1">
+        <v>4</v>
+      </c>
+      <c r="R7" s="1">
+        <v>2</v>
+      </c>
+      <c r="S7" s="1">
+        <v>8</v>
+      </c>
+      <c r="T7" s="1">
+        <v>3</v>
+      </c>
+      <c r="U7" s="1">
+        <v>27</v>
+      </c>
+      <c r="V7" s="1">
+        <v>4</v>
+      </c>
+      <c r="W7" s="1">
+        <v>64</v>
+      </c>
+      <c r="X7" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="1">
+        <v>97</v>
+      </c>
+      <c r="J8" s="1">
+        <v>64</v>
+      </c>
+      <c r="K8" s="1">
+        <v>67</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1">
+        <v>3</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S8" s="1">
+        <v>97</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U8" s="1">
+        <v>77</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W8" s="1">
+        <v>46</v>
+      </c>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+    </row>
+    <row r="9" spans="1:25" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
+      <c r="C9" s="1">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q4">
+      <c r="Q9" s="1">
         <v>3</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T4" s="1" t="s">
+      <c r="U9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U4" t="s">
-        <v>15</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="W4" t="s">
+      <c r="W9" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
-      </c>
-      <c r="K5">
-        <v>16</v>
-      </c>
-      <c r="L5" t="s">
-        <v>54</v>
-      </c>
-      <c r="O5" s="1"/>
-      <c r="Q5">
-        <v>4</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <v>8</v>
-      </c>
-      <c r="U5">
-        <v>141</v>
-      </c>
-      <c r="V5">
-        <v>10</v>
-      </c>
-      <c r="W5">
-        <v>226</v>
-      </c>
-      <c r="X5">
-        <v>15</v>
-      </c>
-      <c r="Y5">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="L6" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q6">
-        <v>4</v>
-      </c>
-      <c r="R6">
-        <v>2</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="T6">
-        <v>3</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V6">
-        <v>5</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="X6">
-        <v>25</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>4</v>
-      </c>
-      <c r="I7">
-        <v>8</v>
-      </c>
-      <c r="J7">
-        <v>27</v>
-      </c>
-      <c r="K7">
-        <v>64</v>
-      </c>
-      <c r="L7" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q7">
-        <v>4</v>
-      </c>
-      <c r="R7">
-        <v>2</v>
-      </c>
-      <c r="S7">
-        <v>8</v>
-      </c>
-      <c r="T7">
-        <v>3</v>
-      </c>
-      <c r="U7">
-        <v>27</v>
-      </c>
-      <c r="V7">
-        <v>4</v>
-      </c>
-      <c r="W7">
-        <v>64</v>
-      </c>
-      <c r="X7">
-        <v>10</v>
-      </c>
-      <c r="Y7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" t="s">
-        <v>64</v>
-      </c>
-      <c r="I8">
-        <v>97</v>
-      </c>
-      <c r="J8">
-        <v>64</v>
-      </c>
-      <c r="K8">
-        <v>67</v>
-      </c>
-      <c r="L8" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q8">
-        <v>3</v>
-      </c>
-      <c r="R8" t="s">
-        <v>61</v>
-      </c>
-      <c r="S8">
-        <v>97</v>
-      </c>
-      <c r="T8" t="s">
-        <v>65</v>
-      </c>
-      <c r="U8">
-        <v>77</v>
-      </c>
-      <c r="V8" t="s">
-        <v>66</v>
-      </c>
-      <c r="W8">
-        <v>46</v>
-      </c>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>